<commit_message>
i18n and validateion issues are updated. * labels should be defined as property style but class getter/setter. * i18n instance is now kept in ValidateConfig class statically.
</commit_message>
<xml_diff>
--- a/meta/labels/en/ChartSampleEn.xlsx
+++ b/meta/labels/en/ChartSampleEn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yhaino/Desktop/dapanda-front-core/meta/labels/en/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/labels/en/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D6E4DE-8ABF-0D4D-8AE7-A91E92358A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2BB075-107D-E546-92DA-04A712CBEC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2980" yWindow="900" windowWidth="25820" windowHeight="14980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="config" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">valueObject!$B$51:$B$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">valueObject!$B$52:$B$74</definedName>
     <definedName name="accessScope">config!$B$4:$B$6</definedName>
     <definedName name="accessScope2">config!$B$4:$B$5</definedName>
     <definedName name="adjustDefaultValue">config!$N$4:$N$5</definedName>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>画面ラベル定義書</t>
   </si>
@@ -270,6 +270,23 @@
   </si>
   <si>
     <t>"language"</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>ラベル</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>/* TypeScript 独自。インタフェイス指定が優先します。 */</t>
+    <rPh sb="14" eb="16">
+      <t xml:space="preserve">ドクジ </t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t xml:space="preserve">シテイガ </t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t xml:space="preserve">ユウセｎ </t>
+    </rPh>
     <phoneticPr fontId="6"/>
   </si>
 </sst>
@@ -1198,10 +1215,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMJ90"/>
+  <dimension ref="A1:AMJ91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1376,146 +1393,147 @@
       </c>
     </row>
     <row r="18" spans="1:9" s="16" customFormat="1">
-      <c r="A18" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
+      <c r="A18" s="76" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="76"/>
+      <c r="C18" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="19" spans="1:9" s="16" customFormat="1">
       <c r="A19" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="21"/>
     </row>
     <row r="20" spans="1:9" s="16" customFormat="1">
       <c r="A20" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21"/>
+    </row>
+    <row r="21" spans="1:9" s="16" customFormat="1">
+      <c r="A21" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="16" customFormat="1">
-      <c r="A21" s="76" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="76"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="16" t="s">
+    </row>
+    <row r="22" spans="1:9" s="16" customFormat="1">
+      <c r="A22" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="76"/>
+      <c r="C22" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="9"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-    </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="29"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="25"/>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="9"/>
+      <c r="A25" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="28"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="9"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="9"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
       <c r="E27" s="9"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="30" t="s">
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B30" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="9"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="33"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
       <c r="I30" s="9"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="33"/>
       <c r="B31" s="34"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="38"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="36"/>
       <c r="E31" s="9"/>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
@@ -1523,10 +1541,10 @@
       <c r="I31" s="9"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="39"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="42"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="38"/>
       <c r="E32" s="9"/>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
@@ -1534,58 +1552,58 @@
       <c r="I32" s="9"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="9"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
       <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="9"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="30" t="s">
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="25"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B36" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="33"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
       <c r="I36" s="9"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="33"/>
       <c r="B37" s="34"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="38"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="36"/>
       <c r="E37" s="9"/>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
@@ -1593,10 +1611,10 @@
       <c r="I37" s="9"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="39"/>
-      <c r="B38" s="40"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="42"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="38"/>
       <c r="E38" s="9"/>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
@@ -1604,61 +1622,61 @@
       <c r="I38" s="9"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="43"/>
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="9"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="43"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="30" t="s">
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="25"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B42" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="9"/>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="33">
+      <c r="C42" s="31"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="33">
         <v>1</v>
       </c>
-      <c r="B42" s="34" t="s">
+      <c r="B43" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="35"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="9"/>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="33"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="38"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="36"/>
       <c r="E43" s="9"/>
       <c r="F43" s="22"/>
       <c r="G43" s="22"/>
@@ -1666,10 +1684,10 @@
       <c r="I43" s="9"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="39"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="42"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="38"/>
       <c r="E44" s="9"/>
       <c r="F44" s="22"/>
       <c r="G44" s="22"/>
@@ -1677,90 +1695,81 @@
       <c r="I44" s="9"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="43"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B46" s="44"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="45"/>
-    </row>
-    <row r="47" spans="1:9" ht="13.5" customHeight="1">
-      <c r="A47" s="77" t="s">
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="45"/>
+    </row>
+    <row r="48" spans="1:9" ht="13.5" customHeight="1">
+      <c r="A48" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="77" t="s">
+      <c r="B48" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="73" t="s">
+      <c r="C48" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="D47" s="73" t="s">
+      <c r="D48" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="E47" s="73" t="s">
+      <c r="E48" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="F47" s="73"/>
-      <c r="G47" s="46"/>
-      <c r="H47" s="47"/>
-      <c r="I47" s="48"/>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="77"/>
-      <c r="B48" s="77"/>
-      <c r="C48" s="73"/>
-      <c r="D48" s="73"/>
-      <c r="E48" s="73"/>
       <c r="F48" s="73"/>
-      <c r="G48" s="49"/>
-      <c r="H48" s="50"/>
-      <c r="I48" s="45"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
+      <c r="I48" s="48"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="33">
-        <v>1</v>
-      </c>
-      <c r="B49" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="C49" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="D49" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="E49" s="53"/>
-      <c r="F49" s="54"/>
-      <c r="G49" s="54"/>
-      <c r="H49" s="55"/>
+      <c r="A49" s="77"/>
+      <c r="B49" s="77"/>
+      <c r="C49" s="73"/>
+      <c r="D49" s="73"/>
+      <c r="E49" s="73"/>
+      <c r="F49" s="73"/>
+      <c r="G49" s="49"/>
+      <c r="H49" s="50"/>
       <c r="I49" s="45"/>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="33">
-        <f t="shared" ref="A50:A81" si="0">A49+1</f>
-        <v>2</v>
-      </c>
-      <c r="B50" s="56" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="B50" s="51" t="s">
+        <v>50</v>
       </c>
       <c r="C50" s="52" t="s">
         <v>51</v>
       </c>
       <c r="D50" s="53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E50" s="53"/>
       <c r="F50" s="54"/>
@@ -1770,62 +1779,68 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="33">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" ref="A51:A82" si="0">A50+1</f>
+        <v>2</v>
       </c>
       <c r="B51" s="56" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C51" s="52" t="s">
         <v>51</v>
       </c>
       <c r="D51" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="E51" s="57"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="59"/>
+        <v>61</v>
+      </c>
+      <c r="E51" s="53"/>
+      <c r="F51" s="54"/>
+      <c r="G51" s="54"/>
+      <c r="H51" s="55"/>
       <c r="I51" s="45"/>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="33">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B52" s="56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C52" s="52" t="s">
         <v>51</v>
       </c>
       <c r="D52" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="E52" s="53"/>
-      <c r="F52" s="54"/>
-      <c r="G52" s="54"/>
-      <c r="H52" s="60"/>
+        <v>56</v>
+      </c>
+      <c r="E52" s="57"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="59"/>
       <c r="I52" s="45"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="33">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B53" s="56"/>
-      <c r="C53" s="52"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="57"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="59"/>
+        <v>4</v>
+      </c>
+      <c r="B53" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="D53" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="E53" s="53"/>
+      <c r="F53" s="54"/>
+      <c r="G53" s="54"/>
+      <c r="H53" s="60"/>
       <c r="I53" s="45"/>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="33">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B54" s="56"/>
       <c r="C54" s="52"/>
@@ -1839,35 +1854,35 @@
     <row r="55" spans="1:9">
       <c r="A55" s="33">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B55" s="70"/>
+        <v>6</v>
+      </c>
+      <c r="B55" s="56"/>
       <c r="C55" s="52"/>
-      <c r="D55" s="72"/>
-      <c r="E55" s="53"/>
-      <c r="F55" s="54"/>
-      <c r="G55" s="54"/>
-      <c r="H55" s="60"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="57"/>
+      <c r="F55" s="58"/>
+      <c r="G55" s="58"/>
+      <c r="H55" s="59"/>
       <c r="I55" s="45"/>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="33">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B56" s="56"/>
-      <c r="C56" s="71"/>
-      <c r="D56" s="53"/>
-      <c r="E56" s="57"/>
-      <c r="F56" s="58"/>
-      <c r="G56" s="58"/>
-      <c r="H56" s="59"/>
+        <v>7</v>
+      </c>
+      <c r="B56" s="70"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="72"/>
+      <c r="E56" s="53"/>
+      <c r="F56" s="54"/>
+      <c r="G56" s="54"/>
+      <c r="H56" s="60"/>
       <c r="I56" s="45"/>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="33">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B57" s="56"/>
       <c r="C57" s="71"/>
@@ -1881,35 +1896,35 @@
     <row r="58" spans="1:9">
       <c r="A58" s="33">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B58" s="56"/>
       <c r="C58" s="71"/>
       <c r="D58" s="53"/>
-      <c r="E58" s="53"/>
-      <c r="F58" s="54"/>
-      <c r="G58" s="54"/>
-      <c r="H58" s="60"/>
+      <c r="E58" s="57"/>
+      <c r="F58" s="58"/>
+      <c r="G58" s="58"/>
+      <c r="H58" s="59"/>
       <c r="I58" s="45"/>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="33">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B59" s="56"/>
-      <c r="C59" s="52"/>
+      <c r="C59" s="71"/>
       <c r="D59" s="53"/>
-      <c r="E59" s="57"/>
-      <c r="F59" s="58"/>
-      <c r="G59" s="58"/>
-      <c r="H59" s="59"/>
+      <c r="E59" s="53"/>
+      <c r="F59" s="54"/>
+      <c r="G59" s="54"/>
+      <c r="H59" s="60"/>
       <c r="I59" s="45"/>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="33">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B60" s="56"/>
       <c r="C60" s="52"/>
@@ -1923,7 +1938,7 @@
     <row r="61" spans="1:9">
       <c r="A61" s="33">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B61" s="56"/>
       <c r="C61" s="52"/>
@@ -1937,49 +1952,49 @@
     <row r="62" spans="1:9">
       <c r="A62" s="33">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B62" s="56"/>
       <c r="C62" s="52"/>
       <c r="D62" s="53"/>
-      <c r="E62" s="53"/>
-      <c r="F62" s="54"/>
-      <c r="G62" s="54"/>
-      <c r="H62" s="60"/>
+      <c r="E62" s="57"/>
+      <c r="F62" s="58"/>
+      <c r="G62" s="58"/>
+      <c r="H62" s="59"/>
       <c r="I62" s="45"/>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="33">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B63" s="56"/>
       <c r="C63" s="52"/>
       <c r="D63" s="53"/>
-      <c r="E63" s="57"/>
-      <c r="F63" s="58"/>
-      <c r="G63" s="58"/>
-      <c r="H63" s="59"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="54"/>
+      <c r="G63" s="54"/>
+      <c r="H63" s="60"/>
       <c r="I63" s="45"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="33">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B64" s="56"/>
       <c r="C64" s="52"/>
       <c r="D64" s="53"/>
-      <c r="E64" s="53"/>
-      <c r="F64" s="54"/>
-      <c r="G64" s="54"/>
-      <c r="H64" s="55"/>
+      <c r="E64" s="57"/>
+      <c r="F64" s="58"/>
+      <c r="G64" s="58"/>
+      <c r="H64" s="59"/>
       <c r="I64" s="45"/>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="33">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B65" s="56"/>
       <c r="C65" s="52"/>
@@ -1987,13 +2002,13 @@
       <c r="E65" s="53"/>
       <c r="F65" s="54"/>
       <c r="G65" s="54"/>
-      <c r="H65" s="60"/>
+      <c r="H65" s="55"/>
       <c r="I65" s="45"/>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="33">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B66" s="56"/>
       <c r="C66" s="52"/>
@@ -2007,7 +2022,7 @@
     <row r="67" spans="1:9">
       <c r="A67" s="33">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B67" s="56"/>
       <c r="C67" s="52"/>
@@ -2021,7 +2036,7 @@
     <row r="68" spans="1:9">
       <c r="A68" s="33">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B68" s="56"/>
       <c r="C68" s="52"/>
@@ -2035,7 +2050,7 @@
     <row r="69" spans="1:9">
       <c r="A69" s="33">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B69" s="56"/>
       <c r="C69" s="52"/>
@@ -2049,7 +2064,7 @@
     <row r="70" spans="1:9">
       <c r="A70" s="33">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B70" s="56"/>
       <c r="C70" s="52"/>
@@ -2063,7 +2078,7 @@
     <row r="71" spans="1:9">
       <c r="A71" s="33">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B71" s="56"/>
       <c r="C71" s="52"/>
@@ -2077,7 +2092,7 @@
     <row r="72" spans="1:9">
       <c r="A72" s="33">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B72" s="56"/>
       <c r="C72" s="52"/>
@@ -2091,7 +2106,7 @@
     <row r="73" spans="1:9">
       <c r="A73" s="33">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B73" s="56"/>
       <c r="C73" s="52"/>
@@ -2099,13 +2114,13 @@
       <c r="E73" s="53"/>
       <c r="F73" s="54"/>
       <c r="G73" s="54"/>
-      <c r="H73" s="55"/>
+      <c r="H73" s="60"/>
       <c r="I73" s="45"/>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="33">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B74" s="56"/>
       <c r="C74" s="52"/>
@@ -2119,49 +2134,49 @@
     <row r="75" spans="1:9">
       <c r="A75" s="33">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B75" s="56"/>
       <c r="C75" s="52"/>
       <c r="D75" s="53"/>
-      <c r="E75" s="57"/>
-      <c r="F75" s="58"/>
-      <c r="G75" s="58"/>
-      <c r="H75" s="59"/>
+      <c r="E75" s="53"/>
+      <c r="F75" s="54"/>
+      <c r="G75" s="54"/>
+      <c r="H75" s="55"/>
       <c r="I75" s="45"/>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="33">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B76" s="56"/>
       <c r="C76" s="52"/>
       <c r="D76" s="53"/>
-      <c r="E76" s="53"/>
-      <c r="F76" s="54"/>
-      <c r="G76" s="54"/>
-      <c r="H76" s="60"/>
+      <c r="E76" s="57"/>
+      <c r="F76" s="58"/>
+      <c r="G76" s="58"/>
+      <c r="H76" s="59"/>
       <c r="I76" s="45"/>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="33">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B77" s="56"/>
       <c r="C77" s="52"/>
       <c r="D77" s="53"/>
-      <c r="E77" s="57"/>
-      <c r="F77" s="58"/>
-      <c r="G77" s="58"/>
-      <c r="H77" s="59"/>
+      <c r="E77" s="53"/>
+      <c r="F77" s="54"/>
+      <c r="G77" s="54"/>
+      <c r="H77" s="60"/>
       <c r="I77" s="45"/>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="33">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B78" s="56"/>
       <c r="C78" s="52"/>
@@ -2175,39 +2190,39 @@
     <row r="79" spans="1:9">
       <c r="A79" s="33">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B79" s="56"/>
       <c r="C79" s="52"/>
       <c r="D79" s="53"/>
-      <c r="E79" s="53"/>
-      <c r="F79" s="54"/>
-      <c r="G79" s="54"/>
-      <c r="H79" s="60"/>
+      <c r="E79" s="57"/>
+      <c r="F79" s="58"/>
+      <c r="G79" s="58"/>
+      <c r="H79" s="59"/>
       <c r="I79" s="45"/>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="33">
         <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B80" s="70"/>
-      <c r="C80" s="71"/>
-      <c r="D80" s="72"/>
-      <c r="E80" s="57"/>
-      <c r="F80" s="58"/>
-      <c r="G80" s="58"/>
-      <c r="H80" s="59"/>
+        <v>31</v>
+      </c>
+      <c r="B80" s="56"/>
+      <c r="C80" s="52"/>
+      <c r="D80" s="53"/>
+      <c r="E80" s="53"/>
+      <c r="F80" s="54"/>
+      <c r="G80" s="54"/>
+      <c r="H80" s="60"/>
       <c r="I80" s="45"/>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="33">
         <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B81" s="56"/>
+        <v>32</v>
+      </c>
+      <c r="B81" s="70"/>
       <c r="C81" s="71"/>
-      <c r="D81" s="53"/>
+      <c r="D81" s="72"/>
       <c r="E81" s="57"/>
       <c r="F81" s="58"/>
       <c r="G81" s="58"/>
@@ -2215,25 +2230,28 @@
       <c r="I81" s="45"/>
     </row>
     <row r="82" spans="1:9">
-      <c r="A82" s="33"/>
+      <c r="A82" s="33">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
       <c r="B82" s="56"/>
       <c r="C82" s="71"/>
       <c r="D82" s="53"/>
-      <c r="E82" s="53"/>
-      <c r="F82" s="54"/>
-      <c r="G82" s="54"/>
-      <c r="H82" s="60"/>
+      <c r="E82" s="57"/>
+      <c r="F82" s="58"/>
+      <c r="G82" s="58"/>
+      <c r="H82" s="59"/>
       <c r="I82" s="45"/>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="33"/>
       <c r="B83" s="56"/>
-      <c r="C83" s="52"/>
+      <c r="C83" s="71"/>
       <c r="D83" s="53"/>
-      <c r="E83" s="57"/>
-      <c r="F83" s="58"/>
-      <c r="G83" s="58"/>
-      <c r="H83" s="59"/>
+      <c r="E83" s="53"/>
+      <c r="F83" s="54"/>
+      <c r="G83" s="54"/>
+      <c r="H83" s="60"/>
       <c r="I83" s="45"/>
     </row>
     <row r="84" spans="1:9">
@@ -2263,10 +2281,10 @@
       <c r="B86" s="56"/>
       <c r="C86" s="52"/>
       <c r="D86" s="53"/>
-      <c r="E86" s="53"/>
-      <c r="F86" s="54"/>
-      <c r="G86" s="54"/>
-      <c r="H86" s="60"/>
+      <c r="E86" s="57"/>
+      <c r="F86" s="58"/>
+      <c r="G86" s="58"/>
+      <c r="H86" s="59"/>
       <c r="I86" s="45"/>
     </row>
     <row r="87" spans="1:9">
@@ -2274,10 +2292,10 @@
       <c r="B87" s="56"/>
       <c r="C87" s="52"/>
       <c r="D87" s="53"/>
-      <c r="E87" s="57"/>
-      <c r="F87" s="58"/>
-      <c r="G87" s="58"/>
-      <c r="H87" s="59"/>
+      <c r="E87" s="53"/>
+      <c r="F87" s="54"/>
+      <c r="G87" s="54"/>
+      <c r="H87" s="60"/>
       <c r="I87" s="45"/>
     </row>
     <row r="88" spans="1:9">
@@ -2285,10 +2303,10 @@
       <c r="B88" s="56"/>
       <c r="C88" s="52"/>
       <c r="D88" s="53"/>
-      <c r="E88" s="53"/>
-      <c r="F88" s="54"/>
-      <c r="G88" s="54"/>
-      <c r="H88" s="55"/>
+      <c r="E88" s="57"/>
+      <c r="F88" s="58"/>
+      <c r="G88" s="58"/>
+      <c r="H88" s="59"/>
       <c r="I88" s="45"/>
     </row>
     <row r="89" spans="1:9">
@@ -2299,12 +2317,12 @@
       <c r="E89" s="53"/>
       <c r="F89" s="54"/>
       <c r="G89" s="54"/>
-      <c r="H89" s="60"/>
+      <c r="H89" s="55"/>
       <c r="I89" s="45"/>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="33"/>
-      <c r="B90" s="52"/>
+      <c r="B90" s="56"/>
       <c r="C90" s="52"/>
       <c r="D90" s="53"/>
       <c r="E90" s="53"/>
@@ -2313,29 +2331,41 @@
       <c r="H90" s="60"/>
       <c r="I90" s="45"/>
     </row>
+    <row r="91" spans="1:9">
+      <c r="A91" s="33"/>
+      <c r="B91" s="52"/>
+      <c r="C91" s="52"/>
+      <c r="D91" s="53"/>
+      <c r="E91" s="53"/>
+      <c r="F91" s="54"/>
+      <c r="G91" s="54"/>
+      <c r="H91" s="60"/>
+      <c r="I91" s="45"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="E47:F48"/>
+  <mergeCells count="10">
+    <mergeCell ref="E48:F49"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
   </mergeCells>
   <phoneticPr fontId="6"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D90" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D91" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20:C21" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21:C22" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustFiledName</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>createToString</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2343,11 +2373,11 @@
       <formula1>accessScope2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16:C17" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16:C18" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>isAbstract</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>isFinal</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>